<commit_message>
Added latest tests to worksheet
</commit_message>
<xml_diff>
--- a/experiments/UCI-20-SSDP-ACOxSSDPxNMEEFxMESDIFxSDIGA-Tabelaov4.xlsx
+++ b/experiments/UCI-20-SSDP-ACOxSSDPxNMEEFxMESDIFxSDIGA-Tabelaov4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13035" activeTab="4"/>
+    <workbookView windowWidth="28710" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -206,10 +206,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -228,6 +228,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -235,29 +250,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -272,7 +275,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,14 +298,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,9 +312,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -317,32 +326,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -350,9 +343,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -364,11 +357,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -411,7 +411,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,19 +495,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,91 +549,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,43 +567,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,11 +651,47 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,8 +699,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -684,17 +720,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -707,59 +748,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -771,130 +771,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6075,11 +6075,11 @@
   <dimension ref="A1:AD101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C63" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomRight" activeCell="E77" sqref="D77:E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -15407,7 +15407,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="H2" sqref="H2:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -16570,8 +16570,8 @@
   <sheetPr/>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -18896,7 +18896,7 @@
   <sheetPr/>
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>